<commit_message>
Updated examples, should have everything to develop new code now
</commit_message>
<xml_diff>
--- a/data-raw/data3CIA-ebV-logl.xlsx
+++ b/data-raw/data3CIA-ebV-logl.xlsx
@@ -8,15 +8,17 @@
   <sheets>
     <sheet name="e(b)" sheetId="1" r:id="rId2"/>
     <sheet name="e(V)" sheetId="2" r:id="rId4"/>
-    <sheet name="family" sheetId="3" r:id="rId5"/>
+    <sheet name="cmd" sheetId="3" r:id="rId5"/>
     <sheet name="cmdline" sheetId="4" r:id="rId6"/>
+    <sheet name="family" sheetId="5" r:id="rId7"/>
+    <sheet name="frm" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="25" uniqueCount="17">
   <si>
     <t>y1</t>
   </si>
@@ -57,10 +59,16 @@
     <t>var(_cons[cohort])</t>
   </si>
   <si>
+    <t>mestreg</t>
+  </si>
+  <si>
+    <t>mestreg c.age c.fev1pp ib0.mmrc || cohort: , dist(loglogistic) time</t>
+  </si>
+  <si>
     <t>loglogistic</t>
   </si>
   <si>
-    <t>mestreg c.age c.fev1pp ib0.mmrc || cohort: , dist(loglogistic) time</t>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -577,4 +585,38 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>